<commit_message>
Aggiornamento del file report-checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#DOCPLANNERSRLXX/Docplanner/GipoLisFSE/1/report-checklist.xlsx
+++ b/GATEWAY/A1#111#DOCPLANNERSRLXX/Docplanner/GipoLisFSE/1/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\Desktop\TEMP\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\Desktop\TEMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C97E1042-261A-4139-8F1B-1B8FC1AB1086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F8BAF4-D0E7-4A9C-A590-DFD8A4B528C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="511" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="180">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -364,22 +364,7 @@
     </r>
   </si>
   <si>
-    <t>2025-11-13T17:06:14Z</t>
-  </si>
-  <si>
-    <t>23c41a0ebba8c15e86b17836d757f1b3</t>
-  </si>
-  <si>
-    <t>UNKNOWN_WORKFLOW_ID</t>
-  </si>
-  <si>
-    <t>Campo token JWT non valido.Il campo purpose_of_use non è valorizzatocode. 403</t>
-  </si>
-  <si>
     <t>NO</t>
-  </si>
-  <si>
-    <t>Gestito dal BackOffice attraverso LogSystem -&gt; Rigenerazione Certificato</t>
   </si>
   <si>
     <t>KO</t>
@@ -434,12 +419,6 @@
     </r>
   </si>
   <si>
-    <t>7529cbeea95e93086e9e953764d5f71e</t>
-  </si>
-  <si>
-    <t>Campo token JWT non valido.Il campo action_id non è correttocode. 403</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_LAB_TIMEOUT</t>
   </si>
   <si>
@@ -825,6 +804,15 @@
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>L’applicazione controlla la presenza dell'action_id non conforme. Non potrà mai verificarsi questo caso. L'applicazione non effettuerà mai la chiamata per questa casistica</t>
+  </si>
+  <si>
+    <t>L’applicazione setta automaticamente il valore predefinto ‘TREATMENT’ in mancanza del purposeOfUse inviato</t>
+  </si>
+  <si>
+    <t>Docplanner</t>
   </si>
 </sst>
 </file>
@@ -2889,10 +2877,10 @@
   <dimension ref="A1:W586"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10:XFD26"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2938,7 +2926,9 @@
         <v>18</v>
       </c>
       <c r="B2" s="48"/>
-      <c r="C2" s="49"/>
+      <c r="C2" s="49" t="s">
+        <v>179</v>
+      </c>
       <c r="D2" s="48"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -3086,7 +3076,7 @@
       <c r="V7" s="2"/>
       <c r="W7" s="9"/>
     </row>
-    <row r="8" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -3106,7 +3096,7 @@
       <c r="V8" s="2"/>
       <c r="W8" s="9"/>
     </row>
-    <row r="9" spans="1:23" s="18" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" s="18" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>23</v>
       </c>
@@ -3177,7 +3167,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33">
         <v>4</v>
       </c>
@@ -3224,7 +3214,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="35">
         <v>28</v>
       </c>
@@ -3240,52 +3230,32 @@
       <c r="E11" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="37">
-        <v>45974.71266203704</v>
-      </c>
-      <c r="G11" s="37" t="s">
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="H11" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="I11" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="J11" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="K11" s="38"/>
+      <c r="K11" s="38" t="s">
+        <v>177</v>
+      </c>
       <c r="L11" s="38"/>
-      <c r="M11" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="N11" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="O11" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="P11" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q11" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="R11" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="S11" s="38" t="s">
-        <v>62</v>
-      </c>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="38"/>
       <c r="T11" s="38"/>
       <c r="U11" s="39"/>
       <c r="V11" s="40"/>
       <c r="W11" s="38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="35">
         <v>36</v>
       </c>
@@ -3296,57 +3266,37 @@
         <v>47</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E12" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="37">
-        <v>45974.71266203704</v>
-      </c>
-      <c r="G12" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="H12" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="I12" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="J12" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="K12" s="38"/>
+      <c r="K12" s="38" t="s">
+        <v>178</v>
+      </c>
       <c r="L12" s="38"/>
-      <c r="M12" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="N12" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="O12" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="P12" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q12" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="R12" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="S12" s="38" t="s">
-        <v>62</v>
-      </c>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="38"/>
       <c r="T12" s="38"/>
       <c r="U12" s="39"/>
       <c r="V12" s="40"/>
       <c r="W12" s="38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="35">
         <v>44</v>
       </c>
@@ -3357,10 +3307,10 @@
         <v>47</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E13" s="43" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
@@ -3378,28 +3328,28 @@
         <v>53</v>
       </c>
       <c r="O13" s="38" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="P13" s="38" t="s">
         <v>53</v>
       </c>
       <c r="Q13" s="38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="R13" s="38" t="s">
         <v>53</v>
       </c>
       <c r="S13" s="38" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="T13" s="38"/>
       <c r="U13" s="39"/>
       <c r="V13" s="40"/>
       <c r="W13" s="38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35">
         <v>53</v>
       </c>
@@ -3410,22 +3360,22 @@
         <v>47</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E14" s="43" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F14" s="37">
         <v>45974.712650462963</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="H14" s="37" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="I14" s="42" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="J14" s="38" t="s">
         <v>53</v>
@@ -3439,28 +3389,28 @@
         <v>53</v>
       </c>
       <c r="O14" s="38" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="P14" s="38" t="s">
         <v>53</v>
       </c>
       <c r="Q14" s="38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="R14" s="38" t="s">
         <v>53</v>
       </c>
       <c r="S14" s="38" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="T14" s="38"/>
       <c r="U14" s="39"/>
       <c r="V14" s="40"/>
       <c r="W14" s="38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="35">
         <v>55</v>
       </c>
@@ -3471,22 +3421,22 @@
         <v>47</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E15" s="43" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F15" s="37">
         <v>45974.712650462963</v>
       </c>
       <c r="G15" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="H15" s="37" t="s">
-        <v>81</v>
-      </c>
       <c r="I15" s="42" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="J15" s="38" t="s">
         <v>53</v>
@@ -3500,28 +3450,28 @@
         <v>53</v>
       </c>
       <c r="O15" s="38" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="P15" s="38" t="s">
         <v>53</v>
       </c>
       <c r="Q15" s="38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="R15" s="38" t="s">
         <v>53</v>
       </c>
       <c r="S15" s="38" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="T15" s="38"/>
       <c r="U15" s="39"/>
       <c r="V15" s="40"/>
       <c r="W15" s="38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="35">
         <v>56</v>
       </c>
@@ -3532,22 +3482,22 @@
         <v>47</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E16" s="43" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F16" s="37">
         <v>45974.712500000001</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H16" s="37" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I16" s="42" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="J16" s="38" t="s">
         <v>53</v>
@@ -3561,28 +3511,28 @@
         <v>53</v>
       </c>
       <c r="O16" s="38" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="P16" s="38" t="s">
         <v>53</v>
       </c>
       <c r="Q16" s="38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="R16" s="38" t="s">
         <v>53</v>
       </c>
       <c r="S16" s="38" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="T16" s="38"/>
       <c r="U16" s="39"/>
       <c r="V16" s="40"/>
       <c r="W16" s="38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="35">
         <v>57</v>
       </c>
@@ -3593,22 +3543,22 @@
         <v>47</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E17" s="43" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F17" s="37">
         <v>45974.712511574071</v>
       </c>
       <c r="G17" s="37" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H17" s="37" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="I17" s="42" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="J17" s="38" t="s">
         <v>53</v>
@@ -3622,28 +3572,28 @@
         <v>53</v>
       </c>
       <c r="O17" s="38" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="P17" s="38" t="s">
         <v>53</v>
       </c>
       <c r="Q17" s="38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="R17" s="38" t="s">
         <v>53</v>
       </c>
       <c r="S17" s="38" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="T17" s="38"/>
       <c r="U17" s="39"/>
       <c r="V17" s="40"/>
       <c r="W17" s="38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="35">
         <v>59</v>
       </c>
@@ -3654,22 +3604,22 @@
         <v>47</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E18" s="43" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F18" s="37">
         <v>45974.712604166663</v>
       </c>
       <c r="G18" s="37" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H18" s="37" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="I18" s="42" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="J18" s="38" t="s">
         <v>53</v>
@@ -3683,28 +3633,28 @@
         <v>53</v>
       </c>
       <c r="O18" s="38" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="P18" s="38" t="s">
         <v>53</v>
       </c>
       <c r="Q18" s="38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="R18" s="38" t="s">
         <v>53</v>
       </c>
       <c r="S18" s="38" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="T18" s="38"/>
       <c r="U18" s="39"/>
       <c r="V18" s="40"/>
       <c r="W18" s="38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="35">
         <v>60</v>
       </c>
@@ -3715,22 +3665,22 @@
         <v>47</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E19" s="43" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="F19" s="37">
         <v>45974.712604166663</v>
       </c>
       <c r="G19" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="I19" s="42" t="s">
         <v>98</v>
-      </c>
-      <c r="H19" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="I19" s="42" t="s">
-        <v>105</v>
       </c>
       <c r="J19" s="38" t="s">
         <v>53</v>
@@ -3744,28 +3694,28 @@
         <v>53</v>
       </c>
       <c r="O19" s="38" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P19" s="38" t="s">
         <v>53</v>
       </c>
       <c r="Q19" s="38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="R19" s="38" t="s">
         <v>53</v>
       </c>
       <c r="S19" s="38" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="T19" s="38"/>
       <c r="U19" s="39"/>
       <c r="V19" s="40"/>
       <c r="W19" s="38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="35">
         <v>61</v>
       </c>
@@ -3776,22 +3726,22 @@
         <v>47</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E20" s="43" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="F20" s="37">
         <v>45974.712604166663</v>
       </c>
       <c r="G20" s="37" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H20" s="37" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="I20" s="42" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="J20" s="38" t="s">
         <v>53</v>
@@ -3805,28 +3755,28 @@
         <v>53</v>
       </c>
       <c r="O20" s="38" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="P20" s="38" t="s">
         <v>53</v>
       </c>
       <c r="Q20" s="38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="R20" s="38" t="s">
         <v>53</v>
       </c>
       <c r="S20" s="38" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="T20" s="38"/>
       <c r="U20" s="39"/>
       <c r="V20" s="40"/>
       <c r="W20" s="38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="35">
         <v>62</v>
       </c>
@@ -3837,22 +3787,22 @@
         <v>47</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E21" s="43" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F21" s="37">
         <v>45974.71261574074</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H21" s="37" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="I21" s="42" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="J21" s="38" t="s">
         <v>53</v>
@@ -3866,28 +3816,28 @@
         <v>53</v>
       </c>
       <c r="O21" s="38" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="P21" s="38" t="s">
         <v>53</v>
       </c>
       <c r="Q21" s="38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="R21" s="38" t="s">
         <v>53</v>
       </c>
       <c r="S21" s="38" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="T21" s="38"/>
       <c r="U21" s="39"/>
       <c r="V21" s="40"/>
       <c r="W21" s="38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="35">
         <v>191</v>
       </c>
@@ -3898,23 +3848,23 @@
         <v>47</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="F22" s="37"/>
       <c r="G22" s="37"/>
       <c r="H22" s="37"/>
       <c r="I22" s="42"/>
       <c r="J22" s="38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K22" s="38" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="L22" s="38" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="M22" s="38"/>
       <c r="N22" s="38"/>
@@ -3930,7 +3880,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35">
         <v>376</v>
       </c>
@@ -3941,23 +3891,23 @@
         <v>47</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E23" s="43" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F23" s="37"/>
       <c r="G23" s="37"/>
       <c r="H23" s="37"/>
       <c r="I23" s="42"/>
       <c r="J23" s="38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K23" s="38" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="L23" s="38" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="M23" s="38"/>
       <c r="N23" s="38"/>
@@ -3973,7 +3923,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="35">
         <v>452</v>
       </c>
@@ -3984,22 +3934,22 @@
         <v>47</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E24" s="43" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F24" s="37">
         <v>45974.712453703702</v>
       </c>
       <c r="G24" s="37" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="H24" s="37" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="I24" s="42" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="J24" s="38" t="s">
         <v>53</v>
@@ -4020,7 +3970,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="35">
         <v>466</v>
       </c>
@@ -4031,22 +3981,22 @@
         <v>47</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E25" s="44" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="F25" s="35">
         <v>45974.712465277778</v>
       </c>
       <c r="G25" s="35" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="H25" s="35" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="I25" s="35" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="J25" s="38" t="s">
         <v>53</v>
@@ -4060,28 +4010,28 @@
         <v>53</v>
       </c>
       <c r="O25" s="38" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="P25" s="38" t="s">
         <v>53</v>
       </c>
       <c r="Q25" s="38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="R25" s="38" t="s">
         <v>53</v>
       </c>
       <c r="S25" s="38" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="T25" s="38"/>
       <c r="U25" s="35"/>
       <c r="V25" s="35"/>
       <c r="W25" s="35" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="35">
         <v>473</v>
       </c>
@@ -4092,22 +4042,22 @@
         <v>47</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E26" s="43" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F26" s="37">
         <v>45974.71261574074</v>
       </c>
       <c r="G26" s="37" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H26" s="37" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="I26" s="42" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="J26" s="38" t="s">
         <v>53</v>
@@ -4121,25 +4071,25 @@
         <v>53</v>
       </c>
       <c r="O26" s="38" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="P26" s="38" t="s">
         <v>53</v>
       </c>
       <c r="Q26" s="38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="R26" s="38" t="s">
         <v>53</v>
       </c>
       <c r="S26" s="38" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="T26" s="38"/>
       <c r="U26" s="39"/>
       <c r="V26" s="40"/>
       <c r="W26" s="38" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8212,42 +8162,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -8277,22 +8227,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8300,139 +8250,139 @@
         <v>47</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>159</v>
-      </c>
       <c r="D4" s="31" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9418,7 +9368,7 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>53</v>
@@ -9426,10 +9376,10 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10443,15 +10393,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -10709,7 +10650,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
@@ -10721,15 +10662,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10748,7 +10690,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -10765,6 +10707,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>